<commit_message>
Updated normalization flagging and check_missing function
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A33818-AC57-48B4-A567-48BA7CCA749B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B72B1-A90D-4286-A8DF-F1D558E28875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34635" yWindow="2385" windowWidth="21600" windowHeight="11325" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22365" windowHeight="11055" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -337,6 +337,60 @@
   </si>
   <si>
     <t>Soft Stop (Clowder Doc Missing)</t>
+  </si>
+  <si>
+    <t>missing_required_test_substance_chemical_info</t>
+  </si>
+  <si>
+    <t>Missing required test substance chemical information</t>
+  </si>
+  <si>
+    <t>age_category_match_error</t>
+  </si>
+  <si>
+    <t>Error with age category matching</t>
+  </si>
+  <si>
+    <t>conc_conversion_needed_percentage</t>
+  </si>
+  <si>
+    <t>conc_conversion_needed_radioactive</t>
+  </si>
+  <si>
+    <t>conc_conversion_needed_rate</t>
+  </si>
+  <si>
+    <t>missing_conc_original_values</t>
+  </si>
+  <si>
+    <t>missing_dose_level_values</t>
+  </si>
+  <si>
+    <t>missing_height_values</t>
+  </si>
+  <si>
+    <t>missing_time_original_values</t>
+  </si>
+  <si>
+    <t>Missing required time field</t>
+  </si>
+  <si>
+    <t>Missing required dose field</t>
+  </si>
+  <si>
+    <t>Missing required concentration field</t>
+  </si>
+  <si>
+    <t>Missing height values</t>
+  </si>
+  <si>
+    <t>Conversion logic needed for radioactive concentration units</t>
+  </si>
+  <si>
+    <t>Conversion logic needed for concentration rate units</t>
+  </si>
+  <si>
+    <t>Template has percentage concentration units that need conversion for normalization</t>
   </si>
 </sst>
 </file>
@@ -688,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,8 +1250,107 @@
         <v>99</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C45" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
+  <autoFilter ref="A1:C54" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated template and flag map
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B72B1-A90D-4286-A8DF-F1D558E28875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFDC9DA-F2EF-4109-B53D-6814E73011A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22365" windowHeight="11055" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
+    <workbookView xWindow="5760" yWindow="3324" windowWidth="17280" windowHeight="8964" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -391,6 +391,12 @@
   </si>
   <si>
     <t>Template has percentage concentration units that need conversion for normalization</t>
+  </si>
+  <si>
+    <t>missing_administration_term_units</t>
+  </si>
+  <si>
+    <t>Missing administration term units for conversion</t>
   </si>
 </sst>
 </file>
@@ -742,20 +748,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -766,7 +772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -777,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -788,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -799,7 +805,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -810,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -821,7 +827,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -832,7 +838,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -843,7 +849,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -854,7 +860,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -865,7 +871,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -876,7 +882,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -887,7 +893,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -898,7 +904,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -909,7 +915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -920,7 +926,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -931,7 +937,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -942,415 +948,426 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>67</v>
       </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>71</v>
       </c>
-      <c r="C34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>73</v>
       </c>
-      <c r="C35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>74</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>75</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="C38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>80</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="C39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>83</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>84</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>85</v>
       </c>
-      <c r="C41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>87</v>
       </c>
-      <c r="C42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>88</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>89</v>
       </c>
-      <c r="C43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>90</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>91</v>
       </c>
-      <c r="C44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>97</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>98</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>101</v>
       </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>102</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>103</v>
       </c>
-      <c r="C47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>117</v>
       </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>105</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>115</v>
       </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>106</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>116</v>
       </c>
-      <c r="C50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>109</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>114</v>
       </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>107</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>108</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>112</v>
       </c>
-      <c r="C53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>110</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>111</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C54" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
+  <autoFilter ref="A1:C55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to code and dictionaries to fit new PKWG PCB dataset conversions
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFDC9DA-F2EF-4109-B53D-6814E73011A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3324" windowWidth="17280" windowHeight="8964" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
+    <workbookView xWindow="5295" yWindow="885" windowWidth="16635" windowHeight="8160" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="123">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -397,6 +397,15 @@
   </si>
   <si>
     <t>Missing administration term units for conversion</t>
+  </si>
+  <si>
+    <t>empty_sheet</t>
+  </si>
+  <si>
+    <t>Loaded template has empty sheet</t>
+  </si>
+  <si>
+    <t>Hard Stop (Empty Sheet)</t>
   </si>
 </sst>
 </file>
@@ -748,20 +757,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -772,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -783,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -794,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -805,7 +814,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -816,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -827,7 +836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -838,7 +847,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -849,7 +858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -860,7 +869,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -871,7 +880,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -882,7 +891,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -893,7 +902,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -904,7 +913,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -915,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -926,7 +935,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -937,7 +946,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -948,7 +957,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -959,7 +968,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -970,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -981,7 +990,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1003,7 +1012,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1014,7 +1023,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1190,7 +1199,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -1267,7 +1276,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -1278,7 +1287,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -1289,7 +1298,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -1311,7 +1320,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -1333,7 +1342,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -1344,7 +1353,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -1355,7 +1364,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -1364,6 +1373,17 @@
       </c>
       <c r="C55" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated template and required fields check.
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7392A9C1-9CAA-443B-A88D-B2901151DDE1}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="885" windowWidth="16635" windowHeight="8160" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -406,6 +406,48 @@
   </si>
   <si>
     <t>Hard Stop (Empty Sheet)</t>
+  </si>
+  <si>
+    <t>file_location</t>
+  </si>
+  <si>
+    <t>Where the file was processed from a "local" file directory or from "clowder" with accompanying Clowder file ID.</t>
+  </si>
+  <si>
+    <t>missing_dose_volume_units</t>
+  </si>
+  <si>
+    <t>missing_dermal_applied_area_units</t>
+  </si>
+  <si>
+    <t>Missing dose_volume units with dose_volume entry</t>
+  </si>
+  <si>
+    <t>Missing dermal_applied_area units with dermal_applied_area entry</t>
+  </si>
+  <si>
+    <t>missing_aerosol_particle_density_units</t>
+  </si>
+  <si>
+    <t>Missing aerosol_particle_density units with aerosol_particle_density entry</t>
+  </si>
+  <si>
+    <t>missing_age_units</t>
+  </si>
+  <si>
+    <t>Missing age units with age entry</t>
+  </si>
+  <si>
+    <t>missing_height_units</t>
+  </si>
+  <si>
+    <t>Missing height units with height entry</t>
+  </si>
+  <si>
+    <t>missing_conc_bound_type</t>
+  </si>
+  <si>
+    <t>Missing conc_bound_type when a bound entry is present</t>
   </si>
 </sst>
 </file>
@@ -757,20 +799,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -781,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -792,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -803,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -814,7 +856,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -825,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -836,7 +878,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -847,7 +889,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -858,7 +900,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -869,7 +911,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -880,7 +922,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -891,7 +933,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -902,7 +944,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -913,7 +955,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -924,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -935,7 +977,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -946,7 +988,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -957,7 +999,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -968,7 +1010,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -979,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -990,7 +1032,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1001,7 +1043,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1012,7 +1054,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1023,7 +1065,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1034,7 +1076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1045,7 +1087,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1056,7 +1098,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1067,7 +1109,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1078,7 +1120,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1089,7 +1131,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1100,7 +1142,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1111,7 +1153,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1122,7 +1164,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1133,7 +1175,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1144,7 +1186,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1155,7 +1197,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1166,7 +1208,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1177,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1188,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1199,7 +1241,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1210,7 +1252,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1221,7 +1263,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -1232,7 +1274,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -1243,7 +1285,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1254,7 +1296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1265,7 +1307,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -1276,7 +1318,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -1287,7 +1329,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -1298,7 +1340,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -1309,7 +1351,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -1320,7 +1362,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -1331,7 +1373,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -1342,7 +1384,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -1353,7 +1395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -1364,7 +1406,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -1375,7 +1417,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -1384,6 +1426,83 @@
       </c>
       <c r="C56" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Normalize directly from database with all fields intact. Improved qc_flag reporting to sheet/table.
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7392A9C1-9CAA-443B-A88D-B2901151DDE1}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{623E6A08-517D-422B-98B0-4AC1638A2EE1}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -448,6 +448,27 @@
   </si>
   <si>
     <t>Missing conc_bound_type when a bound entry is present</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Studies</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>Conc_Time_Values</t>
   </si>
 </sst>
 </file>
@@ -799,714 +820,904 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
       <c r="B18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" t="s">
         <v>119</v>
       </c>
-      <c r="C18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
       <c r="B20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
       <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
       <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
       <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
       <c r="B25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
       <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
       <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
       <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
       <c r="B29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
       <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
       <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
         <v>63</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
       <c r="B32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" t="s">
         <v>65</v>
       </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
       <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
         <v>67</v>
       </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>68</v>
       </c>
       <c r="B34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
       <c r="B35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" t="s">
         <v>71</v>
       </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>72</v>
       </c>
       <c r="B36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" t="s">
         <v>73</v>
       </c>
-      <c r="C36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
       <c r="B37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" t="s">
         <v>75</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
       <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" t="s">
         <v>77</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
       <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="s">
         <v>79</v>
       </c>
-      <c r="C39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
       <c r="B40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" t="s">
         <v>81</v>
       </c>
-      <c r="C40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
       <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" t="s">
         <v>83</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
       <c r="B42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" t="s">
         <v>85</v>
       </c>
-      <c r="C42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
       <c r="B43" t="s">
+        <v>141</v>
+      </c>
+      <c r="C43" t="s">
         <v>87</v>
       </c>
-      <c r="C43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
       <c r="B44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" t="s">
         <v>89</v>
       </c>
-      <c r="C44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
       <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
         <v>91</v>
       </c>
-      <c r="C45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
       <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" t="s">
         <v>98</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>100</v>
       </c>
       <c r="B47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" t="s">
         <v>101</v>
       </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>102</v>
       </c>
       <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="s">
         <v>103</v>
       </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>104</v>
       </c>
       <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
         <v>117</v>
       </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>105</v>
       </c>
       <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
         <v>115</v>
       </c>
-      <c r="C50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
       <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
         <v>116</v>
       </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>109</v>
       </c>
       <c r="B52" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" t="s">
         <v>114</v>
       </c>
-      <c r="C52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>107</v>
       </c>
       <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" t="s">
         <v>113</v>
       </c>
-      <c r="C53" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>108</v>
       </c>
       <c r="B54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" t="s">
         <v>112</v>
       </c>
-      <c r="C54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>110</v>
       </c>
       <c r="B55" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" t="s">
         <v>111</v>
       </c>
-      <c r="C55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>120</v>
       </c>
       <c r="B56" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" t="s">
         <v>121</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>123</v>
       </c>
       <c r="B57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
       <c r="B58" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" t="s">
         <v>127</v>
       </c>
-      <c r="C58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>126</v>
       </c>
       <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>129</v>
       </c>
       <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" t="s">
         <v>130</v>
       </c>
-      <c r="C60" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>131</v>
       </c>
       <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" t="s">
         <v>132</v>
       </c>
-      <c r="C61" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>133</v>
       </c>
       <c r="B62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" t="s">
         <v>134</v>
       </c>
-      <c r="C62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>135</v>
       </c>
       <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" t="s">
         <v>136</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
+  <autoFilter ref="A1:D55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
First case of adding qc_flags by record ID.
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{623E6A08-517D-422B-98B0-4AC1638A2EE1}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53678688-2246-42DB-B547-1C3FDB9922CE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="145">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>Conc_Time_Values</t>
+  </si>
+  <si>
+    <t>species_not_normalized</t>
   </si>
 </sst>
 </file>
@@ -820,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,6 +1719,20 @@
         <v>92</v>
       </c>
     </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
qc_flag blanks to NA
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53678688-2246-42DB-B547-1C3FDB9922CE}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B7971FE-A694-4C51-A31D-DE8F25434881}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="148">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -472,6 +472,15 @@
   </si>
   <si>
     <t>species_not_normalized</t>
+  </si>
+  <si>
+    <t>missing_weight_values</t>
+  </si>
+  <si>
+    <t>Subject record missing weight value</t>
+  </si>
+  <si>
+    <t>Soft Stop (Missing Preferred Column)</t>
   </si>
 </sst>
 </file>
@@ -823,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,6 +1742,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix conc character combine, add flag entries.
</commit_message>
<xml_diff>
--- a/input/dictionaries/flag_map.xlsx
+++ b/input/dictionaries/flag_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B7971FE-A694-4C51-A31D-DE8F25434881}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{1B687E25-785E-4B3C-AA07-6EA469B7E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC7C8C93-1B8F-4533-AF0E-593481EE1723}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFA763D9-B2A5-457D-ACD7-9812D7B708A7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
   <si>
     <t>Record Identifier</t>
   </si>
@@ -481,6 +481,27 @@
   </si>
   <si>
     <t>Soft Stop (Missing Preferred Column)</t>
+  </si>
+  <si>
+    <t>negative_conc_lower_bound_values</t>
+  </si>
+  <si>
+    <t>negative_conc_upper_bound_values</t>
+  </si>
+  <si>
+    <t>negative_conc_sd_values</t>
+  </si>
+  <si>
+    <t>cvt_conc_convert_fail</t>
+  </si>
+  <si>
+    <t>Concentration normalization failed</t>
+  </si>
+  <si>
+    <t>cvt_dose_level_normalized_convert_fail</t>
+  </si>
+  <si>
+    <t>Dose normalization failed</t>
   </si>
 </sst>
 </file>
@@ -832,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,97 +1023,97 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>92</v>
@@ -1100,27 +1121,27 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>92</v>
@@ -1128,41 +1149,41 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
         <v>92</v>
@@ -1170,83 +1191,83 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
         <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>96</v>
@@ -1254,13 +1275,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
         <v>96</v>
@@ -1268,27 +1289,27 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
         <v>96</v>
@@ -1296,41 +1317,41 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
         <v>96</v>
@@ -1338,13 +1359,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
         <v>92</v>
@@ -1352,83 +1373,83 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
         <v>141</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
         <v>139</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
         <v>96</v>
@@ -1436,13 +1457,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
         <v>96</v>
@@ -1450,27 +1471,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
         <v>96</v>
@@ -1478,27 +1499,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D47" t="s">
         <v>92</v>
@@ -1506,13 +1527,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
         <v>96</v>
@@ -1520,41 +1541,41 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
         <v>96</v>
@@ -1562,13 +1583,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
         <v>96</v>
@@ -1576,83 +1597,83 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D54" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D55" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D57" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D58" t="s">
         <v>92</v>
@@ -1660,41 +1681,41 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D61" t="s">
         <v>92</v>
@@ -1702,13 +1723,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
         <v>92</v>
@@ -1716,13 +1737,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
         <v>92</v>
@@ -1730,34 +1751,104 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
         <v>139</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B65" t="s">
         <v>139</v>
       </c>
       <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
         <v>146</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D68" t="s">
         <v>147</v>
       </c>
     </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>151</v>
+      </c>
+      <c r="B69" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" t="s">
+        <v>154</v>
+      </c>
+      <c r="D70" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D55" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
+  <autoFilter ref="A1:D58" xr:uid="{1410CAE0-29D8-4088-8086-3C1B59D501A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>